<commit_message>
sorted out clean points, tests of determinant for calibration
</commit_message>
<xml_diff>
--- a/Stereoaufnahmen_Anja/protokollV1.xlsx
+++ b/Stereoaufnahmen_Anja/protokollV1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Programme\Gitkraken\Masterthesis_DuCC\Stereoaufnahmen_Anja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitkraken\Masterthesis_DuCC\Stereoaufnahmen_Anja\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11F6AF0-59CD-430D-9C6E-0D81D5B0167F}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,6 +895,10 @@
       <c r="B30">
         <v>0</v>
       </c>
+      <c r="F30" s="2">
+        <f>D33-D28</f>
+        <v>27264</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">

</xml_diff>